<commit_message>
fix date when import excel in data santri
</commit_message>
<xml_diff>
--- a/public/template/import/template import santri.xlsx
+++ b/public/template/import/template import santri.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bahar\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\panti-asuhan\public\template\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B543F92F-5DE7-4CF6-8FFD-C5A7A8E080CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC93E6A-7A6C-44E2-970A-65043968F744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{01E51AFD-D5D4-4739-AE60-B338B51A58E9}"/>
   </bookViews>
@@ -111,9 +111,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,7 +432,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,11 +441,13 @@
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="20" width="32.140625" bestFit="1" customWidth="1"/>
@@ -466,7 +469,7 @@
       <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G1" t="s">
@@ -481,10 +484,10 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M1" t="s">
@@ -504,9 +507,7 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="F2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>